<commit_message>
UPDATE: Complete Samsung USED pricelist with 36+ models
Added full Samsung USED price coverage:
- Z Fold 3-7 series: $200-$1,620
- Z Flip 4-7 series: $100-$770
- S21 series: $100-$250
- S22 series: $150-$400
- S23 series: $220-$600
- S24 series: $370-$850
- S25 series: $370-$1,100
- A series: $100-$360
- Galaxy Buds 3/Pro: $50-$130

Total: 77 phone models (32 Apple + 36 Samsung + 9 accessories)
Only tablets/watches still use calculated prices (from NEW).
</commit_message>
<xml_diff>
--- a/Samsung_USED_NEW_FULL_REVIEW.xlsx
+++ b/Samsung_USED_NEW_FULL_REVIEW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USED_HIGHEST_ALL" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NEW_HIGHEST_ALL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="USED_HIGHEST_ALL" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="NEW_HIGHEST_ALL" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,13 +18,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -35,7 +38,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,12 +46,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,22 +435,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Storage</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Highest Used Price (SGD)</t>
         </is>
@@ -452,7 +464,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Galaxy Z Flip 7 5G</t>
+          <t>Galaxy Z Fold 3 5G</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -461,7 +473,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -472,7 +484,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Galaxy Z Flip 7 5G</t>
+          <t>Galaxy Z Fold 3 5G</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -481,7 +493,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>650</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4">
@@ -492,16 +504,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Galaxy Z Flip 7 FE 5G</t>
+          <t>Galaxy Z Fold 4 5G</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>128GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>300</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5">
@@ -512,16 +524,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Galaxy Z Flip 7 FE 5G</t>
+          <t>Galaxy Z Fold 4 5G</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>450</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6">
@@ -532,16 +544,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Galaxy Z Fold 7 5G</t>
+          <t>Galaxy Z Fold 4 5G</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1220</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7">
@@ -552,16 +564,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Galaxy Z Fold 7 5G</t>
+          <t>Galaxy Z Fold 5 5G</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1350</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8">
@@ -572,16 +584,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Galaxy Z Fold 7 5G</t>
+          <t>Galaxy Z Fold 5 5G</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1450</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9">
@@ -592,16 +604,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Galaxy A55 5G</t>
+          <t>Galaxy Z Fold 5 5G</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>8/256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>180</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10">
@@ -612,16 +624,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Galaxy A56 5G</t>
+          <t>Galaxy Z Fold 6 5G</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12/256GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>250</v>
+        <v>770</v>
       </c>
     </row>
     <row r="11">
@@ -632,16 +644,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Galaxy A56 5G</t>
+          <t>Galaxy Z Fold 6 5G</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>8/256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>180</v>
+        <v>870</v>
       </c>
     </row>
     <row r="12">
@@ -652,16 +664,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Galaxy S22 Ultra 5G</t>
+          <t>Galaxy Z Fold 6 5G</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>270</v>
+        <v>970</v>
       </c>
     </row>
     <row r="13">
@@ -672,16 +684,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Galaxy S22 Ultra 5G</t>
+          <t>Galaxy Z Fold 7 5G</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>320</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="14">
@@ -692,16 +704,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Galaxy S23 5G</t>
+          <t>Galaxy Z Fold 7 5G</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>250</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="15">
@@ -712,16 +724,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Galaxy S23 FE</t>
+          <t>Galaxy Z Fold 7 5G</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>1TB</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>200</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="16">
@@ -732,16 +744,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Galaxy S23+ 5G</t>
+          <t>Galaxy Z Flip 4 5G</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>330</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17">
@@ -752,16 +764,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Galaxy S23+ 5G</t>
+          <t>Galaxy Z Flip 4 5G</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>370</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18">
@@ -772,16 +784,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Galaxy S23 Ultra 5G</t>
+          <t>Galaxy Z Flip 4 5G</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19">
@@ -792,16 +804,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Galaxy S23 Ultra 5G</t>
+          <t>Galaxy Z Flip 5 5G</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>450</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20">
@@ -812,16 +824,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Galaxy S24 5G</t>
+          <t>Galaxy Z Flip 5 5G</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>380</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21">
@@ -832,16 +844,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Galaxy S24 5G</t>
+          <t>Galaxy Z Flip 6 5G</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>450</v>
+        <v>400</v>
       </c>
     </row>
     <row r="22">
@@ -852,16 +864,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Galaxy S24 FE 5G</t>
+          <t>Galaxy Z Flip 6 5G</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>300</v>
+        <v>450</v>
       </c>
     </row>
     <row r="23">
@@ -872,16 +884,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Galaxy S24 FE 5G</t>
+          <t>Galaxy Z Flip 7 5G</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>256GB</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>360</v>
+        <v>670</v>
       </c>
     </row>
     <row r="24">
@@ -892,16 +904,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Galaxy S24 Plus 5G</t>
+          <t>Galaxy Z Flip 7 5G</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>256GB</t>
+          <t>512GB</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>480</v>
+        <v>770</v>
       </c>
     </row>
     <row r="25">
@@ -912,16 +924,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Galaxy S24 Plus 5G</t>
+          <t>Galaxy Z Flip 7 FE 5G</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>530</v>
+        <v>470</v>
       </c>
     </row>
     <row r="26">
@@ -932,7 +944,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Galaxy S24 Ultra 5G</t>
+          <t>Galaxy Z Flip 7 FE 5G</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -941,7 +953,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>580</v>
+        <v>570</v>
       </c>
     </row>
     <row r="27">
@@ -952,16 +964,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Galaxy S24 Ultra 5G</t>
+          <t>Galaxy S21 5G</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>Base</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>650</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -972,16 +984,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Galaxy S24 Ultra 5G</t>
+          <t>Galaxy S21+ 5G</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>1TB</t>
+          <t>Base</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>700</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29">
@@ -992,7 +1004,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Galaxy S25 5G</t>
+          <t>Galaxy S21 Ultra 5G</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1001,7 +1013,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>560</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30">
@@ -1012,7 +1024,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Galaxy S25 5G</t>
+          <t>Galaxy S21 Ultra 5G</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1021,7 +1033,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>650</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31">
@@ -1032,7 +1044,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Galaxy S25+ 5G</t>
+          <t>Galaxy S21 FE 5G</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1041,7 +1053,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>680</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32">
@@ -1052,16 +1064,16 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Galaxy S25+ 5G</t>
+          <t>Galaxy S22 5G</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>760</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33">
@@ -1072,7 +1084,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Galaxy S25 Ultra 5G</t>
+          <t>Galaxy S22 5G</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1081,7 +1093,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>800</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34">
@@ -1092,16 +1104,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Galaxy S25 Ultra 5G</t>
+          <t>Galaxy S22+ 5G</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>512GB</t>
+          <t>128GB</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>920</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35">
@@ -1112,16 +1124,816 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>Galaxy S22+ 5G</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Galaxy S22 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Galaxy S22 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Galaxy S23 5G</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Galaxy S23 5G</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Galaxy S23+ 5G</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Galaxy S23+ 5G</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Galaxy S23 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Galaxy S23 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Galaxy S23 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Galaxy S23 FE 5G</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Galaxy S24 5G</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Galaxy S24 5G</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Galaxy S24+ 5G</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Galaxy S24+ 5G</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Galaxy S24 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Galaxy S24 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Galaxy S24 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1TB</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Galaxy S24 FE 5G</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Galaxy S24 FE 5G</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Galaxy S25 5G</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Galaxy S25 5G</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Galaxy S25+ 5G</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Galaxy S25+ 5G</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>Galaxy S25 Ultra 5G</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Galaxy S25 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Galaxy S25 Ultra 5G</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
         <is>
           <t>1TB</t>
         </is>
       </c>
-      <c r="D35" t="n">
-        <v>1020</v>
+      <c r="D61" t="n">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Galaxy S25 Edge 5G</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Galaxy S25 Edge 5G</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Galaxy S25 FE 5G</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Galaxy S25 FE 5G</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Galaxy S25 FE 5G</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Galaxy A36 5G</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>8/256GB</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Galaxy A55 5G</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>8/128GB</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Galaxy A55 5G</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>8/256GB</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Galaxy A56 5G</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>12/256GB</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Galaxy A56 5G</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>8/256GB</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Galaxy A73 5G</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>8/128GB</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Galaxy A73 5G</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>8/256GB</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Galaxy Buds 3</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Galaxy Buds 3 Pro</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Base</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1144,22 +1956,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Brand</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Storage</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Highest New Price (SGD)</t>
         </is>

</xml_diff>